<commit_message>
Update es/sig rules code
</commit_message>
<xml_diff>
--- a/data/monthly_es_rules/monthly_significant_rules_biden.xlsx
+++ b/data/monthly_es_rules/monthly_significant_rules_biden.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="202300"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiezd\Documents\GitHub\Reg-Stats\data\monthly_es_rules\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxie\Documents\GitHub\Reg-Stats\data\monthly_es_rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFD2EB4-9C22-405D-9A63-7FE0D281C672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{90C9C651-3028-4297-853F-AC0BAA5E3080}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="25815" windowHeight="13905"/>
   </bookViews>
   <sheets>
     <sheet name="monthly_significant_rules_biden" sheetId="1" r:id="rId1"/>
     <sheet name="Chart" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -54,8 +53,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,6 +649,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1478,6 +1478,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1593,6 +1594,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -1600,7 +1602,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2174,13 +2175,13 @@
 </file>
 
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BDC0AA5C-26FC-45D5-9FE1-E258707DCE04}">
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </chartsheet>
 </file>
@@ -2189,7 +2190,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656972" cy="6285917"/>
+    <xdr:ext cx="8673353" cy="6297706"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -2649,16 +2650,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8482168B-23EE-4241-9CA4-1AEEB8D0C390}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2675,7 +2676,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>44228</v>
       </c>
@@ -2692,7 +2693,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>44256</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>44287</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>44317</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>44348</v>
       </c>
@@ -2760,7 +2761,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>44378</v>
       </c>
@@ -2777,7 +2778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>44409</v>
       </c>
@@ -2794,7 +2795,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>44440</v>
       </c>
@@ -2811,7 +2812,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>44470</v>
       </c>
@@ -2828,7 +2829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>44501</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>44531</v>
       </c>
@@ -2862,7 +2863,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>44562</v>
       </c>
@@ -2879,7 +2880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>44593</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>44621</v>
       </c>
@@ -2913,7 +2914,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>44652</v>
       </c>
@@ -2930,7 +2931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>44682</v>
       </c>
@@ -2947,7 +2948,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>44713</v>
       </c>
@@ -2964,7 +2965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>44743</v>
       </c>
@@ -2981,7 +2982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>44774</v>
       </c>
@@ -2998,7 +2999,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>44805</v>
       </c>
@@ -3015,7 +3016,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>44835</v>
       </c>
@@ -3032,7 +3033,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>44866</v>
       </c>
@@ -3049,7 +3050,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>44896</v>
       </c>
@@ -3066,7 +3067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>44927</v>
       </c>
@@ -3083,7 +3084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>44958</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>44986</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>45017</v>
       </c>
@@ -3134,7 +3135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>45047</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>45078</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>45108</v>
       </c>
@@ -3185,7 +3186,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>45139</v>
       </c>
@@ -3202,7 +3203,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>45170</v>
       </c>
@@ -3219,7 +3220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>45200</v>
       </c>
@@ -3236,7 +3237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>45231</v>
       </c>
@@ -3253,7 +3254,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>45261</v>
       </c>
@@ -3270,7 +3271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>45292</v>
       </c>
@@ -3287,7 +3288,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>45323</v>
       </c>
@@ -3304,7 +3305,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>45352</v>
       </c>
@@ -3321,7 +3322,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>45383</v>
       </c>
@@ -3338,7 +3339,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>45413</v>
       </c>
@@ -3355,7 +3356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>45444</v>
       </c>
@@ -3372,7 +3373,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>45474</v>
       </c>
@@ -3389,7 +3390,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>45505</v>
       </c>
@@ -3406,7 +3407,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>45536</v>
       </c>
@@ -3423,7 +3424,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>45566</v>
       </c>
@@ -3440,7 +3441,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>45597</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>45627</v>
       </c>
@@ -3474,12 +3475,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>45658</v>
       </c>
       <c r="B49">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C49">
         <v>27</v>

</xml_diff>